<commit_message>
all files of my pythin codes
</commit_message>
<xml_diff>
--- a/moms.xlsx
+++ b/moms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me MySelf I\Desktop\desktop prmng\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -35,12 +35,6 @@
     <t>lastname</t>
   </si>
   <si>
-    <t>SINGLE MOM.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\Me MySelf I\Desktop\desktop prmng\New folder</t>
-  </si>
-  <si>
     <t>files path</t>
   </si>
   <si>
@@ -50,21 +44,9 @@
     <t>book cover pdf</t>
   </si>
   <si>
-    <t>moms_book.pdf</t>
-  </si>
-  <si>
     <t>book description</t>
   </si>
   <si>
-    <t xml:space="preserve">Have A Nursing Student That you Would Like to appreciate This coming National Nurses Day. </t>
-  </si>
-  <si>
-    <t>bisac category</t>
-  </si>
-  <si>
-    <t>MED058050</t>
-  </si>
-  <si>
     <t>keywords</t>
   </si>
   <si>
@@ -78,13 +60,51 @@
   </si>
   <si>
     <t>Nursing Degree Loading</t>
+  </si>
+  <si>
+    <t>page-21.pdf</t>
+  </si>
+  <si>
+    <t>C:\PythonProjects</t>
+  </si>
+  <si>
+    <t>ruledbook.pdf</t>
+  </si>
+  <si>
+    <t>A simple gift idea; 120 pages ruled notebook with a glossy finish custom cover. Have A Nursing Student That you Would Like to appreciate. This is a perfect Nursing Student Gift, A 120 page notebook for school.A simple and Inexpensive gift with a custom Quote/ Saying Cover."</t>
+  </si>
+  <si>
+    <t>sta</t>
+  </si>
+  <si>
+    <t>start cover page</t>
+  </si>
+  <si>
+    <t>start book page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>MOT: Master of Occupational Therapy 
+MT-BC: Board Certified Music Therapist
+MMT:  Master of Music Therapy 
+CMA: Certified Medical Assistant 
+RMA: Registered Medical Assistant 
+MA : Medical Assistant 
+CCMA: Certified Clinical Medical Assistant 
+CMAA: Certified Medical Administrative Assistant 
+R.Ph. : Pharmacist 
+CPhT: Certified Pharmacy Technician
+xxxxxxxxxxxxxxxxxxxxxxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +135,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -137,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,6 +180,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -469,16 +500,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
@@ -487,10 +518,11 @@
     <col min="8" max="8" width="22" style="2" customWidth="1"/>
     <col min="9" max="9" width="19" style="2" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="11" width="23.42578125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -501,62 +533,76 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1"/>
+    <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>